<commit_message>
update to parent -2.8.43
</commit_message>
<xml_diff>
--- a/src/main/resources/org/openurp/std/graduation/graduate/ksy_format.xlsx
+++ b/src/main/resources/org/openurp/std/graduation/graduate/ksy_format.xlsx
@@ -133,7 +133,7 @@
     <t>${data.std.gender.name}</t>
   </si>
   <si>
-    <t>${data.std.person.birthday}</t>
+    <t>${data.birthday}</t>
   </si>
   <si>
     <t>${data.std.person.code}</t>
@@ -160,28 +160,27 @@
     <t>${data.std.studyType.name}</t>
   </si>
   <si>
-    <t>${data.std.studyOn}</t>
-  </si>
-  <si>
-    <t>${data.std.graduateOn}</t>
+    <t>${data.studyOn}</t>
+  </si>
+  <si>
+    <t>${data.graduateOn}</t>
   </si>
   <si>
     <t>${data.result.name}</t>
   </si>
   <si>
-    <t>校长</t>
+    <t>${data.president}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="yyyymmdd"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -804,7 +803,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1137,15 +1136,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71681415929203" defaultRowHeight="13.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="8.71681415929203" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="19.0884955752212" customWidth="1"/>
     <col min="2" max="2" width="14.2654867256637" customWidth="1"/>
@@ -1275,6 +1274,11 @@
         <v>35</v>
       </c>
     </row>
+    <row r="3" spans="5:16">
+      <c r="E3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51" footer="0.51"/>
   <headerFooter/>

</xml_diff>